<commit_message>
2021.01.15 class : finished registing excel dumpfile to database
</commit_message>
<xml_diff>
--- a/spring_workspace/FashionShopNew/src/main/webapp/resources/excel/product_dump.xlsx
+++ b/spring_workspace/FashionShopNew/src/main/webapp/resources/excel/product_dump.xlsx
@@ -17,130 +17,130 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <x:si>
+    <x:t>green,purple</x:t>
+  </x:si>
+  <x:si>
+    <x:t>product_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>red,blue,yellow</x:t>
+  </x:si>
+  <x:si>
+    <x:t>subcategory_id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pink,blue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>white,black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>blue,navi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>orange,blue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>filename</x:t>
+  </x:si>
+  <x:si>
+    <x:t>좋아요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ㅋㅋ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>톰보이</x:t>
+  </x:si>
+  <x:si>
+    <x:t>샤넬</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기타</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폴로</x:t>
+  </x:si>
+  <x:si>
+    <x:t>반팔티</x:t>
+  </x:si>
+  <x:si>
+    <x:t>폴햄</x:t>
+  </x:si>
+  <x:si>
+    <x:t>추천함</x:t>
+  </x:si>
+  <x:si>
+    <x:t>red</x:t>
+  </x:si>
+  <x:si>
+    <x:t>price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>XS,S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오리털 점퍼</x:t>
+  </x:si>
+  <x:si>
+    <x:t>brand</x:t>
+  </x:si>
+  <x:si>
+    <x:t>인기니트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>지오지아</x:t>
+  </x:si>
+  <x:si>
+    <x:t>리트머스</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시원해요</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L,XL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S,XXL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>오리털 가디건</x:t>
+  </x:si>
+  <x:si>
+    <x:t>몽클레어</x:t>
+  </x:si>
+  <x:si>
+    <x:t>긴팔티셔츠</x:t>
+  </x:si>
+  <x:si>
     <x:t>temp</x:t>
   </x:si>
   <x:si>
-    <x:t>filename</x:t>
-  </x:si>
-  <x:si>
-    <x:t>추천함</x:t>
-  </x:si>
-  <x:si>
-    <x:t>좋아요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폴햄</x:t>
-  </x:si>
-  <x:si>
-    <x:t>red</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ㅋㅋ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>샤넬</x:t>
-  </x:si>
-  <x:si>
-    <x:t>톰보이</x:t>
-  </x:si>
-  <x:si>
-    <x:t>폴로</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기타</x:t>
-  </x:si>
-  <x:si>
-    <x:t>반팔티</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pink,blue</x:t>
-  </x:si>
-  <x:si>
-    <x:t>white,black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>blue,navi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>orange,blue</x:t>
-  </x:si>
-  <x:si>
-    <x:t>red,blue,yellow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>green,purple</x:t>
-  </x:si>
-  <x:si>
-    <x:t>subcategory_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>product_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>리트머스</x:t>
-  </x:si>
-  <x:si>
-    <x:t>시원해요</x:t>
-  </x:si>
-  <x:si>
-    <x:t>L,XL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>인기니트</x:t>
+    <x:t>닭털 점퍼</x:t>
+  </x:si>
+  <x:si>
+    <x:t>blue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>orange</x:t>
   </x:si>
   <x:si>
     <x:t>제품 좋네요</x:t>
   </x:si>
   <x:si>
-    <x:t>오리털 가디건</x:t>
-  </x:si>
-  <x:si>
-    <x:t>몽클레어</x:t>
-  </x:si>
-  <x:si>
-    <x:t>brand</x:t>
-  </x:si>
-  <x:si>
-    <x:t>긴팔티셔츠</x:t>
-  </x:si>
-  <x:si>
-    <x:t>닭털 점퍼</x:t>
-  </x:si>
-  <x:si>
-    <x:t>지오지아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>S,XXL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>orange</x:t>
-  </x:si>
-  <x:si>
     <x:t>black</x:t>
   </x:si>
   <x:si>
     <x:t>최신니트</x:t>
   </x:si>
   <x:si>
-    <x:t>blue</x:t>
-  </x:si>
-  <x:si>
     <x:t>닭털 가디건</x:t>
   </x:si>
   <x:si>
-    <x:t>price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>XS,S</x:t>
-  </x:si>
-  <x:si>
-    <x:t>오리털 점퍼</x:t>
+    <x:t>따뜻해요</x:t>
   </x:si>
   <x:si>
     <x:t>psize</x:t>
-  </x:si>
-  <x:si>
-    <x:t>따뜻해요</x:t>
   </x:si>
   <x:si>
     <x:t>color</x:t>
@@ -1049,41 +1049,41 @@
   <x:dimension ref="A1:H9"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="150" zoomScaleNormal="150" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="J4" activeCellId="0" sqref="J4:J4"/>
+      <x:selection activeCell="G1" activeCellId="0" sqref="G1:H1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
   <x:cols>
     <x:col min="1" max="1" width="18.875" customWidth="1"/>
     <x:col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="14.3984375" customWidth="1"/>
+    <x:col min="5" max="5" width="14.3984375" customWidth="1"/>
     <x:col min="7" max="7" width="13" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>37</x:v>
-      </x:c>
       <x:c r="D1" s="1" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="E1" s="1" t="s">
-        <x:v>40</x:v>
-      </x:c>
       <x:c r="F1" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G1" s="1" t="s">
         <x:v>44</x:v>
       </x:c>
       <x:c r="H1" s="1" t="s">
-        <x:v>1</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8">
@@ -1091,25 +1091,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C2">
         <x:v>50000</x:v>
       </x:c>
       <x:c r="D2" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E2" t="s">
-        <x:v>38</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="G2" t="s">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="H2" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -1117,25 +1117,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3" t="s">
-        <x:v>36</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C3">
         <x:v>50001</x:v>
       </x:c>
       <x:c r="D3" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E3" t="s">
-        <x:v>22</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F3" t="s">
-        <x:v>4</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G3" t="s">
-        <x:v>24</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H3" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -1143,25 +1143,25 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B4" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C4">
         <x:v>50002</x:v>
       </x:c>
       <x:c r="D4" t="s">
-        <x:v>17</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E4" t="s">
-        <x:v>31</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F4" t="s">
-        <x:v>30</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G4" t="s">
-        <x:v>21</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H4" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8">
@@ -1169,25 +1169,25 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B5" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C5">
         <x:v>50003</x:v>
       </x:c>
       <x:c r="D5" t="s">
-        <x:v>14</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F5" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="F5" t="s">
-        <x:v>26</x:v>
-      </x:c>
       <x:c r="G5" t="s">
-        <x:v>41</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="H5" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8">
@@ -1195,25 +1195,25 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B6" t="s">
-        <x:v>39</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C6">
         <x:v>50004</x:v>
       </x:c>
       <x:c r="D6" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E6" t="s">
-        <x:v>38</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="F6" t="s">
-        <x:v>8</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G6" t="s">
-        <x:v>2</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="H6" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8">
@@ -1221,25 +1221,25 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B7" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C7">
         <x:v>50005</x:v>
       </x:c>
       <x:c r="D7" t="s">
-        <x:v>13</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E7" t="s">
-        <x:v>22</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F7" t="s">
-        <x:v>20</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G7" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H7" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8">
@@ -1256,16 +1256,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E8" t="s">
-        <x:v>31</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F8" t="s">
-        <x:v>7</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G8" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="H8" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8">
@@ -1273,29 +1273,29 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B9" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C9">
         <x:v>50007</x:v>
       </x:c>
       <x:c r="D9" t="s">
-        <x:v>33</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="E9" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F9" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="F9" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="G9" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="H9" t="s">
-        <x:v>0</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="0" copies="1"/>
 </x:worksheet>
 </file>
@@ -1316,7 +1316,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="B2" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
@@ -1324,7 +1324,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="B3" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
@@ -1332,7 +1332,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B4" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
@@ -1340,7 +1340,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B5" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -1348,7 +1348,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B6" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
@@ -1356,7 +1356,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B7" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
@@ -1364,7 +1364,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B8" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
@@ -1372,7 +1372,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B9" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:2">
@@ -1380,7 +1380,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B10" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:2">
@@ -1388,7 +1388,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B11" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:2">
@@ -1396,7 +1396,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B12" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:2">
@@ -1404,7 +1404,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B13" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:2">
@@ -1412,7 +1412,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B14" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:2">
@@ -1420,7 +1420,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B15" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:2">
@@ -1428,7 +1428,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B16" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:2">
@@ -1436,7 +1436,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B17" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:2">
@@ -1444,7 +1444,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B18" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:2">
@@ -1452,7 +1452,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B19" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:2">
@@ -1460,7 +1460,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B20" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:2">
@@ -1468,11 +1468,11 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="B21" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>